<commit_message>
Added updated excel doc
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>Instruction type</t>
   </si>
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F16"/>
+  <dimension ref="A2:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,6 +632,179 @@
         <v>31961</v>
       </c>
     </row>
+    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>3721</v>
+      </c>
+      <c r="D22">
+        <f>B22</f>
+        <v>3721</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f>D22*E22</f>
+        <v>3721</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>298</v>
+      </c>
+      <c r="D23">
+        <f>B23</f>
+        <v>298</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f>D23*E23</f>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>967</v>
+      </c>
+      <c r="D24">
+        <f>B24</f>
+        <v>967</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <f>D24*E24</f>
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>1483</v>
+      </c>
+      <c r="D26">
+        <f>B26-(B30+B31-B25)</f>
+        <v>1391</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <f>D26*E26</f>
+        <v>6955</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>362</v>
+      </c>
+      <c r="D30">
+        <f>B30</f>
+        <v>362</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <f>D30*E30</f>
+        <v>724</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>351</v>
+      </c>
+      <c r="D31">
+        <f>B31</f>
+        <v>351</v>
+      </c>
+      <c r="E31">
+        <v>40</v>
+      </c>
+      <c r="F31">
+        <f>D31*E31</f>
+        <v>14040</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F32" s="4">
+        <f>SUM(F22:F31)</f>
+        <v>27672</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed multiplies to shifts.. shaved off some more time
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="20">
   <si>
     <t>Instruction type</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Commit 2</t>
+  </si>
+  <si>
+    <t>Commit 3</t>
   </si>
 </sst>
 </file>
@@ -450,22 +453,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F49"/>
+  <dimension ref="A2:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -475,12 +478,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -497,7 +500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -516,7 +519,7 @@
         <v>4319</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -535,7 +538,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -554,7 +557,7 @@
         <v>2332</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -562,7 +565,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -581,12 +584,12 @@
         <v>7950</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -594,7 +597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -613,7 +616,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -632,18 +635,18 @@
         <v>16040</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="F16" s="4">
         <f>SUM(F6:F15)</f>
         <v>31961</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -653,12 +656,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>0</v>
       </c>
@@ -675,7 +678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -694,7 +697,7 @@
         <v>3721</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -713,7 +716,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -732,7 +735,7 @@
         <v>1934</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -740,7 +743,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -759,12 +762,12 @@
         <v>6955</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>8</v>
       </c>
@@ -772,7 +775,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -791,7 +794,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -810,18 +813,18 @@
         <v>14040</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="F32" s="4">
         <f>SUM(F22:F31)</f>
         <v>27672</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>16</v>
       </c>
@@ -831,12 +834,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>0</v>
       </c>
@@ -853,7 +856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -872,7 +875,7 @@
         <v>3629</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -891,7 +894,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -910,7 +913,7 @@
         <v>1934</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>4</v>
       </c>
@@ -918,7 +921,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -937,12 +940,12 @@
         <v>6955</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>8</v>
       </c>
@@ -950,7 +953,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -969,7 +972,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -988,10 +991,188 @@
         <v>14040</v>
       </c>
     </row>
-    <row r="49" spans="6:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="F49" s="4">
         <f>SUM(F39:F48)</f>
         <v>27580</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A53" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>3629</v>
+      </c>
+      <c r="D57">
+        <f>B57</f>
+        <v>3629</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57">
+        <f>D57*E57</f>
+        <v>3629</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58">
+        <v>298</v>
+      </c>
+      <c r="D58">
+        <f>B58</f>
+        <v>298</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <f>D58*E58</f>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>967</v>
+      </c>
+      <c r="D59">
+        <f>B59</f>
+        <v>967</v>
+      </c>
+      <c r="E59">
+        <v>2</v>
+      </c>
+      <c r="F59">
+        <f>D59*E59</f>
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>762</v>
+      </c>
+      <c r="D61">
+        <f>B61-(B65+B66-B60)</f>
+        <v>670</v>
+      </c>
+      <c r="E61">
+        <v>5</v>
+      </c>
+      <c r="F61">
+        <f>D61*E61</f>
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65">
+        <v>362</v>
+      </c>
+      <c r="D65">
+        <f>B65</f>
+        <v>362</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65">
+        <f>D65*E65</f>
+        <v>724</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>10</v>
+      </c>
+      <c r="B66">
+        <v>351</v>
+      </c>
+      <c r="D66">
+        <f>B66</f>
+        <v>351</v>
+      </c>
+      <c r="E66">
+        <v>40</v>
+      </c>
+      <c r="F66">
+        <f>D66*E66</f>
+        <v>14040</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="F67" s="4">
+        <f>SUM(F57:F66)</f>
+        <v>23975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shaved a little more off...
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="21">
   <si>
     <t>Instruction type</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Commit 3</t>
+  </si>
+  <si>
+    <t>Commit 4</t>
   </si>
 </sst>
 </file>
@@ -453,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F67"/>
+  <dimension ref="A2:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1175,6 +1178,184 @@
         <v>23975</v>
       </c>
     </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A71" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75">
+        <v>3625</v>
+      </c>
+      <c r="D75">
+        <f>B75</f>
+        <v>3625</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="F75">
+        <f>D75*E75</f>
+        <v>3625</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76">
+        <v>298</v>
+      </c>
+      <c r="D76">
+        <f>B76</f>
+        <v>298</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+      <c r="F76">
+        <f>D76*E76</f>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77">
+        <v>965</v>
+      </c>
+      <c r="D77">
+        <f>B77</f>
+        <v>965</v>
+      </c>
+      <c r="E77">
+        <v>2</v>
+      </c>
+      <c r="F77">
+        <f>D77*E77</f>
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79">
+        <v>761</v>
+      </c>
+      <c r="D79">
+        <f>B79-(B83+B84-B78)</f>
+        <v>669</v>
+      </c>
+      <c r="E79">
+        <v>5</v>
+      </c>
+      <c r="F79">
+        <f>D79*E79</f>
+        <v>3345</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83">
+        <v>361</v>
+      </c>
+      <c r="D83">
+        <f>B83</f>
+        <v>361</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="F83">
+        <f>D83*E83</f>
+        <v>722</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>10</v>
+      </c>
+      <c r="B84">
+        <v>351</v>
+      </c>
+      <c r="D84">
+        <f>B84</f>
+        <v>351</v>
+      </c>
+      <c r="E84">
+        <v>40</v>
+      </c>
+      <c r="F84">
+        <f>D84*E84</f>
+        <v>14040</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="F85" s="4">
+        <f>SUM(F75:F84)</f>
+        <v>23960</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Little lower, but still missing the cache on the inner loop
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="22">
   <si>
     <t>Instruction type</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Commit 4</t>
+  </si>
+  <si>
+    <t>Commit 5</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F85"/>
+  <dimension ref="A2:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1356,6 +1359,184 @@
         <v>23620</v>
       </c>
     </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A88" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A91" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>1</v>
+      </c>
+      <c r="B92">
+        <v>3608</v>
+      </c>
+      <c r="D92">
+        <f>B92</f>
+        <v>3608</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92">
+        <f>D92*E92</f>
+        <v>3608</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>2</v>
+      </c>
+      <c r="B93">
+        <v>72</v>
+      </c>
+      <c r="D93">
+        <f>B93</f>
+        <v>72</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+      <c r="F93">
+        <f>D93*E93</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>3</v>
+      </c>
+      <c r="B94">
+        <v>915</v>
+      </c>
+      <c r="D94">
+        <f>B94</f>
+        <v>915</v>
+      </c>
+      <c r="E94">
+        <v>2</v>
+      </c>
+      <c r="F94">
+        <f>D94*E94</f>
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>4</v>
+      </c>
+      <c r="B95">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96">
+        <v>712</v>
+      </c>
+      <c r="D96">
+        <f>B96-(B100+B101-B95)</f>
+        <v>620</v>
+      </c>
+      <c r="E96">
+        <v>5</v>
+      </c>
+      <c r="F96">
+        <f>D96*E96</f>
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A99" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>9</v>
+      </c>
+      <c r="B100">
+        <v>359</v>
+      </c>
+      <c r="D100">
+        <f>B100</f>
+        <v>359</v>
+      </c>
+      <c r="E100">
+        <v>2</v>
+      </c>
+      <c r="F100">
+        <f>D100*E100</f>
+        <v>718</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>10</v>
+      </c>
+      <c r="B101">
+        <v>350</v>
+      </c>
+      <c r="D101">
+        <f>B101</f>
+        <v>350</v>
+      </c>
+      <c r="E101">
+        <v>40</v>
+      </c>
+      <c r="F101">
+        <f>D101*E101</f>
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="F102" s="4">
+        <f>SUM(F92:F101)</f>
+        <v>23328</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed it so it stores bytes instead of words for better cache performance
Down to 14000 cycles, 85% cache hit
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="24">
   <si>
     <t>Instruction type</t>
   </si>
@@ -83,12 +83,15 @@
   </si>
   <si>
     <t>Commit 6</t>
+  </si>
+  <si>
+    <t>Commit 7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F120"/>
+  <dimension ref="A2:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="G140" sqref="G140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,6 +1721,184 @@
         <v>23007</v>
       </c>
     </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>1</v>
+      </c>
+      <c r="B127">
+        <v>3564</v>
+      </c>
+      <c r="D127">
+        <f>B127</f>
+        <v>3564</v>
+      </c>
+      <c r="E127">
+        <v>1</v>
+      </c>
+      <c r="F127">
+        <f>D127*E127</f>
+        <v>3564</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128">
+        <v>79</v>
+      </c>
+      <c r="D128">
+        <f>B128</f>
+        <v>79</v>
+      </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
+      <c r="F128">
+        <f>D128*E128</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>3</v>
+      </c>
+      <c r="B129">
+        <v>907</v>
+      </c>
+      <c r="D129">
+        <f>B129</f>
+        <v>907</v>
+      </c>
+      <c r="E129">
+        <v>2</v>
+      </c>
+      <c r="F129">
+        <f>D129*E129</f>
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>4</v>
+      </c>
+      <c r="B130">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>5</v>
+      </c>
+      <c r="B131">
+        <v>714</v>
+      </c>
+      <c r="D131">
+        <f>B131-(B135+B136-B130)</f>
+        <v>612</v>
+      </c>
+      <c r="E131">
+        <v>5</v>
+      </c>
+      <c r="F131">
+        <f>D131*E131</f>
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>9</v>
+      </c>
+      <c r="B135">
+        <v>603</v>
+      </c>
+      <c r="D135">
+        <f>B135</f>
+        <v>603</v>
+      </c>
+      <c r="E135">
+        <v>2</v>
+      </c>
+      <c r="F135">
+        <f>D135*E135</f>
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>10</v>
+      </c>
+      <c r="B136">
+        <v>108</v>
+      </c>
+      <c r="D136">
+        <f>B136</f>
+        <v>108</v>
+      </c>
+      <c r="E136">
+        <v>40</v>
+      </c>
+      <c r="F136">
+        <f>D136*E136</f>
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F137" s="4">
+        <f>SUM(F127:F136)</f>
+        <v>14043</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Reduced count by 500
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="25">
   <si>
     <t>Instruction type</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Commit 7</t>
+  </si>
+  <si>
+    <t>Commit 8</t>
   </si>
 </sst>
 </file>
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F137"/>
+  <dimension ref="A2:F154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="G140" sqref="G140"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,6 +1902,184 @@
         <v>14043</v>
       </c>
     </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A140" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F143" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>1</v>
+      </c>
+      <c r="B144">
+        <v>2943</v>
+      </c>
+      <c r="D144">
+        <f>B144</f>
+        <v>2943</v>
+      </c>
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144">
+        <f>D144*E144</f>
+        <v>2943</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>2</v>
+      </c>
+      <c r="B145">
+        <v>72</v>
+      </c>
+      <c r="D145">
+        <f>B145</f>
+        <v>72</v>
+      </c>
+      <c r="E145">
+        <v>1</v>
+      </c>
+      <c r="F145">
+        <f>D145*E145</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>3</v>
+      </c>
+      <c r="B146">
+        <v>915</v>
+      </c>
+      <c r="D146">
+        <f>B146</f>
+        <v>915</v>
+      </c>
+      <c r="E146">
+        <v>2</v>
+      </c>
+      <c r="F146">
+        <f>D146*E146</f>
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>4</v>
+      </c>
+      <c r="B147">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>5</v>
+      </c>
+      <c r="B148">
+        <v>712</v>
+      </c>
+      <c r="D148">
+        <f>B148-(B152+B153-B147)</f>
+        <v>620</v>
+      </c>
+      <c r="E148">
+        <v>5</v>
+      </c>
+      <c r="F148">
+        <f>D148*E148</f>
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>9</v>
+      </c>
+      <c r="B152">
+        <v>599</v>
+      </c>
+      <c r="D152">
+        <f>B152</f>
+        <v>599</v>
+      </c>
+      <c r="E152">
+        <v>2</v>
+      </c>
+      <c r="F152">
+        <f>D152*E152</f>
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>10</v>
+      </c>
+      <c r="B153">
+        <v>110</v>
+      </c>
+      <c r="D153">
+        <f>B153</f>
+        <v>110</v>
+      </c>
+      <c r="E153">
+        <v>40</v>
+      </c>
+      <c r="F153">
+        <f>D153*E153</f>
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F154" s="4">
+        <f>SUM(F144:F153)</f>
+        <v>13543</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Something happened with last commit
This one works. Got it down to ~11000
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="B149" sqref="B149"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,69 +2124,84 @@
       <c r="A163" t="s">
         <v>1</v>
       </c>
+      <c r="B163">
+        <v>2615</v>
+      </c>
       <c r="D163">
         <f>B163</f>
-        <v>0</v>
+        <v>2615</v>
       </c>
       <c r="E163">
         <v>1</v>
       </c>
       <c r="F163">
         <f>D163*E163</f>
-        <v>0</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>2</v>
       </c>
+      <c r="B164">
+        <v>26</v>
+      </c>
       <c r="D164">
         <f>B164</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E164">
         <v>1</v>
       </c>
       <c r="F164">
         <f>D164*E164</f>
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>3</v>
       </c>
+      <c r="B165">
+        <v>762</v>
+      </c>
       <c r="D165">
         <f>B165</f>
-        <v>0</v>
+        <v>762</v>
       </c>
       <c r="E165">
         <v>2</v>
       </c>
       <c r="F165">
         <f>D165*E165</f>
-        <v>0</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>4</v>
       </c>
+      <c r="B166">
+        <v>617</v>
+      </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>5</v>
       </c>
+      <c r="B167">
+        <v>414</v>
+      </c>
       <c r="D167">
         <f>B167-(B171+B172-B166)</f>
-        <v>0</v>
+        <v>322</v>
       </c>
       <c r="E167">
         <v>5</v>
       </c>
       <c r="F167">
         <f>D167*E167</f>
-        <v>0</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -2206,38 +2221,44 @@
       <c r="A171" t="s">
         <v>9</v>
       </c>
+      <c r="B171">
+        <v>599</v>
+      </c>
       <c r="D171">
         <f>B171</f>
-        <v>0</v>
+        <v>599</v>
       </c>
       <c r="E171">
         <v>2</v>
       </c>
       <c r="F171">
         <f>D171*E171</f>
-        <v>0</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>10</v>
       </c>
+      <c r="B172">
+        <v>110</v>
+      </c>
       <c r="D172">
         <f>B172</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="E172">
         <v>40</v>
       </c>
       <c r="F172">
         <f>D172*E172</f>
-        <v>0</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F173" s="4">
         <f>SUM(F163:F172)</f>
-        <v>0</v>
+        <v>11373</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got IC down to 8400
I changed it so the numbers start printing when $t0 is up to 15. This
prevents the check loop from running excessively. Before, it would
increment to 200 before printing, which isn't necessary because all
prime numbers are found much sooner.
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="B190" sqref="B190"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="J199" sqref="J199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2305,69 +2305,84 @@
       <c r="A181" t="s">
         <v>1</v>
       </c>
+      <c r="B181">
+        <v>1998</v>
+      </c>
       <c r="D181">
         <f>B181</f>
-        <v>0</v>
+        <v>1998</v>
       </c>
       <c r="E181">
         <v>1</v>
       </c>
       <c r="F181">
         <f>D181*E181</f>
-        <v>0</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>2</v>
       </c>
+      <c r="B182">
+        <v>6</v>
+      </c>
       <c r="D182">
         <f>B182</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E182">
         <v>1</v>
       </c>
       <c r="F182">
         <f>D182*E182</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>3</v>
       </c>
+      <c r="B183">
+        <v>530</v>
+      </c>
       <c r="D183">
         <f>B183</f>
-        <v>0</v>
+        <v>530</v>
       </c>
       <c r="E183">
         <v>2</v>
       </c>
       <c r="F183">
         <f>D183*E183</f>
-        <v>0</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>4</v>
       </c>
+      <c r="B184">
+        <v>470</v>
+      </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>5</v>
       </c>
+      <c r="B185">
+        <v>352</v>
+      </c>
       <c r="D185">
         <f>B185-(B189+B190-B184)</f>
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="E185">
         <v>5</v>
       </c>
       <c r="F185">
         <f>D185*E185</f>
-        <v>0</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -2387,38 +2402,44 @@
       <c r="A189" t="s">
         <v>9</v>
       </c>
+      <c r="B189">
+        <v>484</v>
+      </c>
       <c r="D189">
         <f>B189</f>
-        <v>0</v>
+        <v>484</v>
       </c>
       <c r="E189">
         <v>2</v>
       </c>
       <c r="F189">
         <f>D189*E189</f>
-        <v>0</v>
+        <v>968</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>10</v>
       </c>
+      <c r="B190">
+        <v>78</v>
+      </c>
       <c r="D190">
         <f>B190</f>
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="E190">
         <v>40</v>
       </c>
       <c r="F190">
         <f>D190*E190</f>
-        <v>0</v>
+        <v>3120</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F191" s="4">
         <f>SUM(F181:F190)</f>
-        <v>0</v>
+        <v>8452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Unrolled the inner loop reducing cycle count to 7422
</commit_message>
<xml_diff>
--- a/running_time.xlsx
+++ b/running_time.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="28">
   <si>
     <t>Instruction type</t>
   </si>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -477,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F209"/>
+  <dimension ref="A2:F226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="B209" sqref="B209"/>
+    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
+      <selection activeCell="I221" sqref="I221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2617,10 +2617,188 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="209" spans="6:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F209" s="4">
         <f>SUM(F199:F208)</f>
         <v>8442</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A212" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B212" s="2"/>
+      <c r="C212" s="2"/>
+      <c r="D212" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A215" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F215" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>1</v>
+      </c>
+      <c r="B216">
+        <v>2009</v>
+      </c>
+      <c r="D216">
+        <f>B216</f>
+        <v>2009</v>
+      </c>
+      <c r="E216">
+        <v>1</v>
+      </c>
+      <c r="F216">
+        <f>D216*E216</f>
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>2</v>
+      </c>
+      <c r="B217">
+        <v>6</v>
+      </c>
+      <c r="D217">
+        <f>B217</f>
+        <v>6</v>
+      </c>
+      <c r="E217">
+        <v>1</v>
+      </c>
+      <c r="F217">
+        <f>D217*E217</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>3</v>
+      </c>
+      <c r="B218">
+        <v>357</v>
+      </c>
+      <c r="D218">
+        <f>B218</f>
+        <v>357</v>
+      </c>
+      <c r="E218">
+        <v>2</v>
+      </c>
+      <c r="F218">
+        <f>D218*E218</f>
+        <v>714</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>4</v>
+      </c>
+      <c r="B219">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>5</v>
+      </c>
+      <c r="B220">
+        <v>181</v>
+      </c>
+      <c r="D220">
+        <f>B220-(B224+B225-B219)</f>
+        <v>89</v>
+      </c>
+      <c r="E220">
+        <v>5</v>
+      </c>
+      <c r="F220">
+        <f>D220*E220</f>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A223" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>9</v>
+      </c>
+      <c r="B224">
+        <v>484</v>
+      </c>
+      <c r="D224">
+        <f>B224</f>
+        <v>484</v>
+      </c>
+      <c r="E224">
+        <v>2</v>
+      </c>
+      <c r="F224">
+        <f>D224*E224</f>
+        <v>968</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>10</v>
+      </c>
+      <c r="B225">
+        <v>82</v>
+      </c>
+      <c r="D225">
+        <f>B225</f>
+        <v>82</v>
+      </c>
+      <c r="E225">
+        <v>40</v>
+      </c>
+      <c r="F225">
+        <f>D225*E225</f>
+        <v>3280</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F226" s="4">
+        <f>SUM(F216:F225)</f>
+        <v>7422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>